<commit_message>
-Überstunden ausrechnen -nur Daten kopieren die nicht schon Kopiert wurden
Signed-off-by: SwissPvP2003 <noahziltener@yahoo.com>
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Projekt-BLJ\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D20D4B6-E12D-4ADA-B915-D9D80783EFCF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CA9C37-9CF9-4305-8334-F12C60A12853}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="597" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1878,7 +1878,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>56.5</c:v>
+                  <c:v>72.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2972,8 +2972,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Y24" sqref="Y24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AT13" sqref="AT13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4251,7 +4251,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>56.5</v>
+        <v>72.5</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -4482,7 +4482,7 @@
       </c>
       <c r="D21" s="83">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E21" s="50"/>
       <c r="F21" s="52">
@@ -4535,8 +4535,12 @@
       <c r="AO21" s="58"/>
       <c r="AP21" s="59"/>
       <c r="AQ21" s="60"/>
-      <c r="AR21" s="55"/>
-      <c r="AS21" s="55"/>
+      <c r="AR21" s="55">
+        <v>2</v>
+      </c>
+      <c r="AS21" s="55">
+        <v>2</v>
+      </c>
       <c r="AT21" s="56"/>
       <c r="AU21" s="57"/>
       <c r="AV21" s="58"/>
@@ -4567,7 +4571,7 @@
       </c>
       <c r="D22" s="83">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E22" s="50"/>
       <c r="F22" s="52">
@@ -4612,8 +4616,12 @@
       <c r="AO22" s="58"/>
       <c r="AP22" s="59"/>
       <c r="AQ22" s="60"/>
-      <c r="AR22" s="55"/>
-      <c r="AS22" s="55"/>
+      <c r="AR22" s="55">
+        <v>2</v>
+      </c>
+      <c r="AS22" s="55">
+        <v>2</v>
+      </c>
       <c r="AT22" s="56"/>
       <c r="AU22" s="57"/>
       <c r="AV22" s="58"/>
@@ -4644,7 +4652,7 @@
       </c>
       <c r="D23" s="83">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E23" s="50"/>
       <c r="F23" s="52">
@@ -4695,8 +4703,12 @@
       <c r="AO23" s="58"/>
       <c r="AP23" s="59"/>
       <c r="AQ23" s="60"/>
-      <c r="AR23" s="61"/>
-      <c r="AS23" s="61"/>
+      <c r="AR23" s="61">
+        <v>2</v>
+      </c>
+      <c r="AS23" s="61">
+        <v>2</v>
+      </c>
       <c r="AT23" s="56"/>
       <c r="AU23" s="57"/>
       <c r="AV23" s="58"/>
@@ -4727,7 +4739,7 @@
       </c>
       <c r="D24" s="83">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E24" s="50"/>
       <c r="F24" s="52">
@@ -4772,8 +4784,12 @@
       <c r="AO24" s="58"/>
       <c r="AP24" s="59"/>
       <c r="AQ24" s="60"/>
-      <c r="AR24" s="55"/>
-      <c r="AS24" s="55"/>
+      <c r="AR24" s="55">
+        <v>2</v>
+      </c>
+      <c r="AS24" s="55">
+        <v>2</v>
+      </c>
       <c r="AT24" s="56"/>
       <c r="AU24" s="57"/>
       <c r="AV24" s="58"/>
@@ -6108,7 +6124,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>68.5</v>
+        <v>84.5</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -6262,11 +6278,11 @@
       </c>
       <c r="AR43" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AS43" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AT43" s="39">
         <f t="shared" si="4"/>
@@ -6440,7 +6456,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>56.5</v>
+        <v>72.5</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>